<commit_message>
Added feadback form links to schedule pages.
</commit_message>
<xml_diff>
--- a/lungradcon/youtube_links/presenter_youtube_links.xlsx
+++ b/lungradcon/youtube_links/presenter_youtube_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamgoode/Desktop/IMPACT_website/IMPACT-Boulder.github.io/lungradcon/youtube_links/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3D6303-6E97-DF43-8D3B-4D705702DAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D150EC5-ADAC-E746-B9A7-8674BD7E44EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35420" yWindow="4420" windowWidth="28040" windowHeight="16620" xr2:uid="{11EE3E19-5510-F24D-83D3-7BAD87BFD821}"/>
+    <workbookView xWindow="-20520" yWindow="2740" windowWidth="19000" windowHeight="20280" xr2:uid="{11EE3E19-5510-F24D-83D3-7BAD87BFD821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Last Name</t>
   </si>
@@ -52,6 +52,69 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=OT49ZApy6Ss&amp;authuser=2</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4HyszYc35ks&amp;authuser=2</t>
+  </si>
+  <si>
+    <t>Fairweather</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Y2RSnJwHHnw</t>
+  </si>
+  <si>
+    <t>Cymes</t>
+  </si>
+  <si>
+    <t>Brittany</t>
+  </si>
+  <si>
+    <t>https://youtu.be/zLBXx2vZERc</t>
+  </si>
+  <si>
+    <t>Easter</t>
+  </si>
+  <si>
+    <t>Parks</t>
+  </si>
+  <si>
+    <t>https://youtu.be/wJFd90i557w</t>
+  </si>
+  <si>
+    <t>Martinot</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=IAGhMZd6Rrg&amp;authuser=2</t>
+  </si>
+  <si>
+    <t>Gimar</t>
+  </si>
+  <si>
+    <t>Caleb</t>
+  </si>
+  <si>
+    <t>https://youtu.be/NVsUoX5tmlw</t>
+  </si>
+  <si>
+    <t>Piskurich</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>https://youtu.be/McZv3w3g8fw</t>
+  </si>
+  <si>
+    <t>Shreekumari</t>
   </si>
 </sst>
 </file>
@@ -424,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BEE5EB-A268-9846-BC7C-0580F5D2AC74}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,6 +522,83 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{CC429765-EC7A-F84B-9116-95F85E0EA66B}"/>

</xml_diff>

<commit_message>
Added youtube links to hidden schedule page.
</commit_message>
<xml_diff>
--- a/lungradcon/youtube_links/presenter_youtube_links.xlsx
+++ b/lungradcon/youtube_links/presenter_youtube_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamgoode/Desktop/IMPACT_website/IMPACT-Boulder.github.io/lungradcon/youtube_links/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D150EC5-ADAC-E746-B9A7-8674BD7E44EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C25071B-C30D-9347-AC31-DC2BCC484369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="2740" windowWidth="19000" windowHeight="20280" xr2:uid="{11EE3E19-5510-F24D-83D3-7BAD87BFD821}"/>
+    <workbookView xWindow="6840" yWindow="860" windowWidth="21080" windowHeight="15140" xr2:uid="{11EE3E19-5510-F24D-83D3-7BAD87BFD821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Last Name</t>
   </si>
@@ -115,6 +115,165 @@
   </si>
   <si>
     <t>Shreekumari</t>
+  </si>
+  <si>
+    <t>On the Schedule</t>
+  </si>
+  <si>
+    <t>Gawronska</t>
+  </si>
+  <si>
+    <t>Aleksandra</t>
+  </si>
+  <si>
+    <t>https://youtu.be/cdqip9iDzEw</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Kloos</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fgNhWlTp3iI</t>
+  </si>
+  <si>
+    <t>Hsing-Ming Chang</t>
+  </si>
+  <si>
+    <t>Jamie</t>
+  </si>
+  <si>
+    <t>https://youtu.be/eQacyfradMY</t>
+  </si>
+  <si>
+    <t>Galinkin</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iwt4gbiIrRQ</t>
+  </si>
+  <si>
+    <t>Bourget</t>
+  </si>
+  <si>
+    <t>Antione</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_mVrVeBKYTo&amp;ab_channel=AntoineBourget</t>
+  </si>
+  <si>
+    <t>Frantzis</t>
+  </si>
+  <si>
+    <t>Constantinos</t>
+  </si>
+  <si>
+    <t>https://youtu.be/w5VG2EgQodk</t>
+  </si>
+  <si>
+    <t>Lolachi</t>
+  </si>
+  <si>
+    <t>Ramin</t>
+  </si>
+  <si>
+    <t>https://youtu.be/UuUktXLQMDo</t>
+  </si>
+  <si>
+    <t>Hendrix</t>
+  </si>
+  <si>
+    <t>Donald</t>
+  </si>
+  <si>
+    <t>https://youtu.be/qcb_nn9RBgo</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>https://youtu.be/xwM3ZIQfqSU</t>
+  </si>
+  <si>
+    <t>Doner</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>https://youtu.be/JH0FZsQb0C8</t>
+  </si>
+  <si>
+    <t>Ayari</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=e5Vtnj_TiR8</t>
+  </si>
+  <si>
+    <t>Lino</t>
+  </si>
+  <si>
+    <t>Gustavo</t>
+  </si>
+  <si>
+    <t>https://youtu.be/juteiMQfDYg</t>
+  </si>
+  <si>
+    <t>Halim</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>https://youtu.be/dcUzcP2EDQ4</t>
+  </si>
+  <si>
+    <t>Tolometti</t>
+  </si>
+  <si>
+    <t>Gavin</t>
+  </si>
+  <si>
+    <t>https://youtu.be/K3QhfR09egQ</t>
+  </si>
+  <si>
+    <t>Fontes</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>https://youtu.be/yrDnJWszz9g</t>
+  </si>
+  <si>
+    <t>Trinh</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>https://youtu.be/CgmLkLtnVMc</t>
+  </si>
+  <si>
+    <t>Shackelford</t>
+  </si>
+  <si>
+    <t>Autum</t>
+  </si>
+  <si>
+    <t>https://youtu.be/yyDC75aNqVE</t>
   </si>
 </sst>
 </file>
@@ -487,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BEE5EB-A268-9846-BC7C-0580F5D2AC74}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,9 +657,10 @@
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="54.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +670,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -521,8 +684,11 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -532,8 +698,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -543,8 +712,11 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -554,8 +726,11 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -565,8 +740,11 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -576,8 +754,11 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -587,8 +768,11 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -597,11 +781,253 @@
       </c>
       <c r="C9" t="s">
         <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{CC429765-EC7A-F84B-9116-95F85E0EA66B}"/>
+    <hyperlink ref="C26" r:id="rId2" xr:uid="{7DC743C6-0C3C-5E44-916C-2370DFAF4902}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added last minute icebreaker slide to hyperlinks on schedule page.
</commit_message>
<xml_diff>
--- a/lungradcon/youtube_links/presenter_youtube_links.xlsx
+++ b/lungradcon/youtube_links/presenter_youtube_links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamgoode/Desktop/IMPACT_website/IMPACT-Boulder.github.io/lungradcon/youtube_links/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamgoode/Desktop/IMPACT_website2/IMPACT-Boulder.github.io/lungradcon/youtube_links/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB1EA5F-F096-2D4C-9D64-32345B6EAC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7D85D-A84C-044B-9C54-D3E837CF1932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="720" windowWidth="21080" windowHeight="15140" xr2:uid="{11EE3E19-5510-F24D-83D3-7BAD87BFD821}"/>
   </bookViews>
@@ -175,9 +175,6 @@
     <t>Constantinos</t>
   </si>
   <si>
-    <t>https://youtu.be/w5VG2EgQodk</t>
-  </si>
-  <si>
     <t>Lolachi</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>https://youtu.be/ufeHYvNQi6k</t>
+  </si>
+  <si>
+    <t>https://youtu.be/2l750_HYBaM</t>
   </si>
 </sst>
 </file>
@@ -668,7 +668,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,7 +883,7 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
         <v>31</v>
@@ -891,13 +891,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>31</v>
@@ -905,13 +905,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>31</v>
@@ -919,13 +919,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
       </c>
       <c r="D18" t="s">
         <v>31</v>
@@ -933,13 +933,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>57</v>
-      </c>
-      <c r="C19" t="s">
-        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>31</v>
@@ -947,13 +947,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>61</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
       </c>
       <c r="D21" t="s">
         <v>31</v>
@@ -975,13 +975,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
         <v>65</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>66</v>
-      </c>
-      <c r="C22" t="s">
-        <v>67</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
@@ -989,13 +989,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>69</v>
-      </c>
-      <c r="C23" t="s">
-        <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -1003,13 +1003,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
         <v>71</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>72</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
       </c>
       <c r="D24" t="s">
         <v>31</v>
@@ -1017,13 +1017,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
         <v>74</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>75</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
       </c>
       <c r="D25" t="s">
         <v>31</v>
@@ -1031,13 +1031,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D26" t="s">
         <v>31</v>
@@ -1045,13 +1045,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
         <v>80</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>81</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
       </c>
       <c r="D27" t="s">
         <v>31</v>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
         <v>83</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
       </c>
       <c r="D28" t="s">
         <v>31</v>

</xml_diff>